<commit_message>
Push avec le travail effectué vendredi dernier, 29.03.19. Modifications légères sur le design, en particulier la zone d'affichage des news. Il est possible de désigner une personne comme responsable de tournoi. La vue qui permet de dupliquer la formule d'un tournoi dans un autre est crée, mais pas fonctionnelle. Quelques commentaires dans le code ont été ajoutés. Lignes superflues supprimées.
</commit_message>
<xml_diff>
--- a/docs/2019-Niels-Pre-TPI/Journal de bord.xlsx
+++ b/docs/2019-Niels-Pre-TPI/Journal de bord.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>Journal de bord</t>
   </si>
@@ -86,13 +86,37 @@
     <t>Maquettes sur Pencil</t>
   </si>
   <si>
-    <t>Test code avec login (news tournoi)</t>
-  </si>
-  <si>
     <t>Difficile à comprendre la doc, Vagrant, etc.</t>
   </si>
   <si>
     <t>BDD complexe</t>
+  </si>
+  <si>
+    <t>Création de la vue news utilisateur</t>
+  </si>
+  <si>
+    <t>Création de la vue news admin et manager</t>
+  </si>
+  <si>
+    <t>Affichage des news dans la vue utilisateur, depuis BDD</t>
+  </si>
+  <si>
+    <t>Enregistrement des news dans la vue manager, dans la BDD</t>
+  </si>
+  <si>
+    <t>Difficulté à comprendre le code orienté objet pour la BDD.</t>
+  </si>
+  <si>
+    <t>Difficulté à insérer des données en orienté objet (Eloquent)</t>
+  </si>
+  <si>
+    <t>Modifications diverses documentation + maquettes</t>
+  </si>
+  <si>
+    <t>Création du code pour désigner un utilisateur comme manager</t>
+  </si>
+  <si>
+    <t>Difficulté à récupérer le nom et prénom, car table intermédiaire</t>
   </si>
 </sst>
 </file>
@@ -195,18 +219,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,248 +515,290 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="37.85546875" customWidth="1"/>
-    <col min="4" max="4" width="54.7109375" customWidth="1"/>
+    <col min="3" max="3" width="65.28515625" customWidth="1"/>
+    <col min="4" max="4" width="65.140625" customWidth="1"/>
     <col min="5" max="5" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>5.03</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="D4" s="2"/>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>6.03</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>6.03</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>8.0299999999999994</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>8.0299999999999994</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8.0299999999999994</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>8.0299999999999994</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>12.03</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>13.03</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
-        <v>6.03</v>
-      </c>
-      <c r="B6" s="6" t="s">
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>14.03</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>15.03</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>19.03</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>20.03</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
-        <v>8.0299999999999994</v>
-      </c>
-      <c r="B7" s="6" t="s">
+      <c r="C16" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>21.03</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
-        <v>8.0299999999999994</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>8.0299999999999994</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <v>8.0299999999999994</v>
-      </c>
-      <c r="B10" s="6" t="s">
+      <c r="C17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="7"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>22.03</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>26.03</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
-        <v>12.03</v>
-      </c>
-      <c r="B11" s="6" t="s">
+      <c r="C19" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>27.03</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
-        <v>13.03</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
-        <v>14.03</v>
-      </c>
-      <c r="B13" s="6" t="s">
+      <c r="C20" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="7"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>28.03</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
-        <v>15.03</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
-        <v>19.03</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>29.03</v>
+      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>

</xml_diff>

<commit_message>
Dernier push. Documentation et journal de bord mis à jour. J'ai également rédigé mon Résumé.
</commit_message>
<xml_diff>
--- a/docs/2019-Niels-Pre-TPI/Journal de bord.xlsx
+++ b/docs/2019-Niels-Pre-TPI/Journal de bord.xlsx
@@ -169,8 +169,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="hh/mm&quot; h&quot;;@"/>
-    <numFmt numFmtId="170" formatCode="[hh]&quot;h &quot;mm&quot; m&quot;;@"/>
+    <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
+    <numFmt numFmtId="165" formatCode="[hh]&quot;h &quot;mm&quot; m&quot;;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -307,24 +307,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,31 +608,31 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="7"/>
-    <col min="2" max="2" width="15" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="103" style="7" customWidth="1"/>
-    <col min="4" max="4" width="65.140625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="76.28515625" style="7" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="7"/>
+    <col min="1" max="1" width="11.42578125" style="6"/>
+    <col min="2" max="2" width="15" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="103" style="6" customWidth="1"/>
+    <col min="4" max="4" width="65.140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="76.28515625" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="17"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -649,7 +649,7 @@
       <c r="A4" s="1">
         <v>5.03</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="11">
         <v>3.125E-2</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -662,7 +662,7 @@
       <c r="A5" s="1">
         <v>6.03</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <v>6.25E-2</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -677,7 +677,7 @@
       <c r="A6" s="1">
         <v>6.03</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="11">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -690,7 +690,7 @@
       <c r="A7" s="1">
         <v>8.0299999999999994</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="11">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -705,7 +705,7 @@
       <c r="A8" s="1">
         <v>8.0299999999999994</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="11">
         <v>0.125</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -720,7 +720,7 @@
       <c r="A9" s="1">
         <v>8.0299999999999994</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="11">
         <v>3.125E-2</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -733,7 +733,7 @@
       <c r="A10" s="1">
         <v>8.0299999999999994</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="11">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -746,7 +746,7 @@
       <c r="A11" s="1">
         <v>12.03</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="11">
         <v>3.125E-2</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -759,7 +759,7 @@
       <c r="A12" s="1">
         <v>13.03</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="11">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -774,7 +774,7 @@
       <c r="A13" s="1">
         <v>13.03</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="11">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -787,7 +787,7 @@
       <c r="A14" s="1">
         <v>14.03</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="11">
         <v>6.25E-2</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -800,7 +800,7 @@
       <c r="A15" s="1">
         <v>14.03</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="11">
         <v>6.25E-2</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -813,7 +813,7 @@
       <c r="A16" s="1">
         <v>14.03</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="11">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -826,14 +826,14 @@
       <c r="A17" s="1">
         <v>14.03</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="11">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="1"/>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="8" t="s">
         <v>35</v>
       </c>
     </row>
@@ -841,33 +841,33 @@
       <c r="A18" s="1">
         <v>15.03</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18" s="11">
         <v>6.25E-2</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D18" s="1"/>
-      <c r="E18" s="9"/>
+      <c r="E18" s="8"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>15.03</v>
       </c>
-      <c r="B19" s="12">
+      <c r="B19" s="11">
         <v>5.2083333333333336E-2</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D19" s="1"/>
-      <c r="E19" s="9"/>
+      <c r="E19" s="8"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>15.03</v>
       </c>
-      <c r="B20" s="12">
+      <c r="B20" s="11">
         <v>0.10416666666666667</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -880,7 +880,7 @@
       <c r="A21" s="1">
         <v>19.03</v>
       </c>
-      <c r="B21" s="12">
+      <c r="B21" s="11">
         <v>3.125E-2</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -893,7 +893,7 @@
       <c r="A22" s="5">
         <v>20.03</v>
       </c>
-      <c r="B22" s="13">
+      <c r="B22" s="12">
         <v>6.25E-2</v>
       </c>
       <c r="C22" s="5" t="s">
@@ -906,7 +906,7 @@
       <c r="A23" s="5">
         <v>21.03</v>
       </c>
-      <c r="B23" s="13">
+      <c r="B23" s="12">
         <v>6.25E-2</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -919,7 +919,7 @@
       <c r="A24" s="5">
         <v>21.03</v>
       </c>
-      <c r="B24" s="13">
+      <c r="B24" s="12">
         <v>0.125</v>
       </c>
       <c r="C24" s="5" t="s">
@@ -934,7 +934,7 @@
       <c r="A25" s="5">
         <v>22.03</v>
       </c>
-      <c r="B25" s="13">
+      <c r="B25" s="12">
         <v>6.25E-2</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -947,7 +947,7 @@
       <c r="A26" s="5">
         <v>22.03</v>
       </c>
-      <c r="B26" s="13">
+      <c r="B26" s="12">
         <v>3.125E-2</v>
       </c>
       <c r="C26" s="5" t="s">
@@ -960,13 +960,13 @@
       <c r="A27" s="5">
         <v>22.03</v>
       </c>
-      <c r="B27" s="13">
+      <c r="B27" s="12">
         <v>0.125</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E27" s="5"/>
@@ -975,7 +975,7 @@
       <c r="A28" s="5">
         <v>26.03</v>
       </c>
-      <c r="B28" s="13">
+      <c r="B28" s="12">
         <v>3.125E-2</v>
       </c>
       <c r="C28" s="5" t="s">
@@ -988,7 +988,7 @@
       <c r="A29" s="5">
         <v>27.03</v>
       </c>
-      <c r="B29" s="13">
+      <c r="B29" s="12">
         <v>6.25E-2</v>
       </c>
       <c r="C29" s="5" t="s">
@@ -997,7 +997,7 @@
       <c r="D29" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="E29" s="8" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1005,33 +1005,33 @@
       <c r="A30" s="5">
         <v>28.03</v>
       </c>
-      <c r="B30" s="13">
+      <c r="B30" s="12">
         <v>5.2083333333333336E-2</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>43</v>
       </c>
       <c r="D30" s="5"/>
-      <c r="E30" s="9"/>
+      <c r="E30" s="8"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
         <v>28.03</v>
       </c>
-      <c r="B31" s="13">
+      <c r="B31" s="12">
         <v>5.2083333333333336E-2</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>45</v>
       </c>
       <c r="D31" s="5"/>
-      <c r="E31" s="9"/>
+      <c r="E31" s="8"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="5">
         <v>29.03</v>
       </c>
-      <c r="B32" s="13">
+      <c r="B32" s="12">
         <v>5.2083333333333336E-2</v>
       </c>
       <c r="C32" s="5" t="s">
@@ -1044,7 +1044,7 @@
       <c r="A33" s="5">
         <v>29.03</v>
       </c>
-      <c r="B33" s="13">
+      <c r="B33" s="12">
         <v>3.125E-2</v>
       </c>
       <c r="C33" s="5" t="s">
@@ -1057,7 +1057,7 @@
       <c r="A34" s="5">
         <v>29.03</v>
       </c>
-      <c r="B34" s="13">
+      <c r="B34" s="12">
         <v>5.2083333333333336E-2</v>
       </c>
       <c r="C34" s="5" t="s">
@@ -1070,7 +1070,7 @@
       <c r="A35" s="5">
         <v>29.03</v>
       </c>
-      <c r="B35" s="13">
+      <c r="B35" s="12">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="C35" s="5" t="s">
@@ -1080,10 +1080,10 @@
       <c r="E35" s="5"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="8">
+      <c r="A36" s="7">
         <v>2.04</v>
       </c>
-      <c r="B36" s="13">
+      <c r="B36" s="12">
         <v>3.125E-2</v>
       </c>
       <c r="C36" s="5" t="s">
@@ -1093,16 +1093,16 @@
       <c r="E36" s="5"/>
     </row>
     <row r="37" spans="1:5" ht="60" x14ac:dyDescent="0.2">
-      <c r="A37" s="8">
+      <c r="A37" s="7">
         <v>3.04</v>
       </c>
-      <c r="B37" s="13">
+      <c r="B37" s="12">
         <v>6.25E-2</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="D37" s="8" t="s">
         <v>29</v>
       </c>
       <c r="E37" s="5"/>
@@ -1111,7 +1111,7 @@
       <c r="A38" s="5">
         <v>4.04</v>
       </c>
-      <c r="B38" s="13">
+      <c r="B38" s="12">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="C38" s="5" t="s">
@@ -1124,7 +1124,7 @@
       <c r="A39" s="5">
         <v>4.04</v>
       </c>
-      <c r="B39" s="13">
+      <c r="B39" s="12">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="C39" s="5" t="s">
@@ -1134,10 +1134,10 @@
       <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="8">
+      <c r="A40" s="7">
         <v>4.04</v>
       </c>
-      <c r="B40" s="13">
+      <c r="B40" s="12">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="C40" s="5" t="s">
@@ -1147,10 +1147,10 @@
       <c r="E40" s="5"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="8">
+      <c r="A41" s="7">
         <v>5.04</v>
       </c>
-      <c r="B41" s="13">
+      <c r="B41" s="12">
         <v>3.125E-2</v>
       </c>
       <c r="C41" s="5" t="s">
@@ -1160,14 +1160,14 @@
       <c r="E41" s="5"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="16"/>
-      <c r="B42" s="15"/>
+      <c r="A42" s="15"/>
+      <c r="B42" s="14"/>
     </row>
     <row r="43" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="17" t="s">
+      <c r="A43" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B43" s="14">
+      <c r="B43" s="13">
         <f>SUM(B4:B41)</f>
         <v>2.1249999999999996</v>
       </c>

</xml_diff>